<commit_message>
added descriptions for flight delay fields
</commit_message>
<xml_diff>
--- a/project2/air-travel-data-dict.xlsx
+++ b/project2/air-travel-data-dict.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="156">
   <si>
     <t>Origin Source</t>
   </si>
@@ -135,10 +135,13 @@
     <t>FLOAT</t>
   </si>
   <si>
+    <t>Number of flights</t>
+  </si>
+  <si>
     <t>arr_del15</t>
   </si>
   <si>
-    <t>Arrival Delay Indicator</t>
+    <t>Difference in minutes between scheduled and actual arrival time</t>
   </si>
   <si>
     <t>carrier_ct</t>
@@ -159,12 +162,21 @@
     <t>arr_cancelled</t>
   </si>
   <si>
+    <t>Number of flights cancelled</t>
+  </si>
+  <si>
     <t>arr_diverted</t>
   </si>
   <si>
+    <t>Number of flights diverted</t>
+  </si>
+  <si>
     <t>arr_delay</t>
   </si>
   <si>
+    <t>Number of flights delayed</t>
+  </si>
+  <si>
     <t>carrier_delay</t>
   </si>
   <si>
@@ -202,6 +214,19 @@
   </si>
   <si>
     <t>Granularity: monthly</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Delay terms defined </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>here</t>
+    </r>
   </si>
   <si>
     <t>https://openflights.org/data</t>
@@ -495,7 +520,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -519,6 +544,16 @@
     </font>
     <font>
       <sz val="10.0"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -537,10 +572,6 @@
       <color rgb="FF222222"/>
       <name val="&quot;Lucida Grande&quot;"/>
     </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -556,13 +587,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDEE2E6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -581,23 +626,29 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1087,135 +1138,152 @@
       <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C15" s="6"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C16" s="6"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C17" s="7"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C18" s="6"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C19" s="6"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C21" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29">
@@ -1225,7 +1293,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32">
@@ -1235,19 +1303,25 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B1"/>
+    <hyperlink r:id="rId2" ref="A35"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1271,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2">
@@ -1279,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3">
@@ -1292,20 +1366,20 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>30</v>
@@ -1313,7 +1387,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
@@ -1321,7 +1395,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -1329,7 +1403,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -1337,7 +1411,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
@@ -1345,18 +1419,18 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -1364,311 +1438,311 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="10"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="7"/>
+      <c r="B18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="10"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="7"/>
+        <v>84</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="10"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="10"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="7"/>
+        <v>85</v>
+      </c>
+      <c r="D21" s="10"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="10"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="7"/>
+        <v>86</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="10"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="7"/>
+        <v>88</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="10"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="7"/>
+        <v>90</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="10"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="7"/>
+        <v>91</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="10"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="7"/>
+        <v>92</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="10"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="7"/>
+        <v>94</v>
+      </c>
+      <c r="D29" s="10"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" s="6" t="s">
+      <c r="A33" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="7"/>
+      <c r="A34" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="10"/>
     </row>
     <row r="35">
-      <c r="A35" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35" s="6" t="s">
+      <c r="A35" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B38" s="6" t="s">
+      <c r="A38" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>99</v>
+      <c r="A39" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B40" s="6" t="s">
+      <c r="A40" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" s="7"/>
+      <c r="A43" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="10"/>
     </row>
     <row r="44">
-      <c r="A44" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D44" s="7"/>
+      <c r="A44" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="10"/>
     </row>
     <row r="45">
-      <c r="A45" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B45" s="9" t="s">
+      <c r="A45" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D45" s="7"/>
+        <v>85</v>
+      </c>
+      <c r="D45" s="10"/>
     </row>
     <row r="46">
-      <c r="A46" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" s="7"/>
+      <c r="A46" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="10"/>
     </row>
     <row r="47">
-      <c r="A47" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B47" s="9" t="s">
+      <c r="A47" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47" s="7"/>
+        <v>85</v>
+      </c>
+      <c r="D47" s="10"/>
     </row>
     <row r="48">
-      <c r="A48" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D48" s="7"/>
+      <c r="A48" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="10"/>
     </row>
     <row r="49">
-      <c r="A49" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>76</v>
+      <c r="A49" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D49" s="7"/>
+        <v>113</v>
+      </c>
+      <c r="D49" s="10"/>
     </row>
     <row r="50">
-      <c r="A50" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B50" s="9" t="s">
+      <c r="A50" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C50" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D50" s="7"/>
+      <c r="C50" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" s="10"/>
     </row>
     <row r="51">
-      <c r="A51" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>112</v>
+      <c r="A51" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="53">
@@ -1678,7 +1752,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56">
@@ -1688,12 +1762,12 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="11" t="s">
-        <v>114</v>
+      <c r="A58" s="8" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1725,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
@@ -1733,7 +1807,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3">
@@ -1746,10 +1820,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6">
@@ -1758,92 +1832,92 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="10"/>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="7"/>
+        <v>126</v>
+      </c>
+      <c r="D9" s="10"/>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D10" s="7"/>
+        <v>128</v>
+      </c>
+      <c r="D10" s="10"/>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>125</v>
+      <c r="A11" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>130</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D11" s="7"/>
+        <v>131</v>
+      </c>
+      <c r="D11" s="10"/>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D12" s="7"/>
+        <v>133</v>
+      </c>
+      <c r="D12" s="10"/>
     </row>
     <row r="13">
-      <c r="A13" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D13" s="7"/>
+        <v>135</v>
+      </c>
+      <c r="D13" s="10"/>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15">
@@ -1856,7 +1930,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19">
@@ -1866,22 +1940,22 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="11" t="s">
-        <v>136</v>
+      <c r="A23" s="8" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1913,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
@@ -1921,7 +1995,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3">
@@ -1937,15 +2011,15 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7">
@@ -1954,85 +2028,85 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="7"/>
+      <c r="A8" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="10"/>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="7"/>
+      <c r="A9" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="10"/>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="7"/>
+      <c r="B10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="7"/>
+      <c r="B11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="10"/>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="7"/>
+      <c r="A12" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13">
-      <c r="A13" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="7"/>
+      <c r="A13" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D14" s="7"/>
+      <c r="A14" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="10"/>
     </row>
     <row r="15">
-      <c r="A15" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17">
@@ -2042,12 +2116,12 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21">
@@ -2057,12 +2131,12 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2103,7 +2177,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">

</xml_diff>